<commit_message>
add E2E test cases
</commit_message>
<xml_diff>
--- a/web/WBTBSsystem/system/downloads/testOut_captain.xlsx
+++ b/web/WBTBSsystem/system/downloads/testOut_captain.xlsx
@@ -486,11 +486,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SG001</t>
+          <t>MY00202</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -499,20 +499,18 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>Scheduled</t>
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45366.68958333333</v>
+        <v>45369.99888888889</v>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" s="2" t="n">
-        <v>45364.81319444445</v>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t xml:space="preserve">NB002
@@ -522,11 +520,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MY001</t>
+          <t>CB0003</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -535,22 +533,21 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>Scheduled</t>
         </is>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>45366.68958333333</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" s="2" t="n">
+        <v>45369.99945601852</v>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve">NB001
-NB002
+          <t xml:space="preserve">NB002
 </t>
         </is>
       </c>

</xml_diff>